<commit_message>
Updating artifacts of the project 02.
</commit_message>
<xml_diff>
--- a/documents/Projeto 02 - RISCV-Decodificação das instruções.xlsx
+++ b/documents/Projeto 02 - RISCV-Decodificação das instruções.xlsx
@@ -5001,11 +5001,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="C46" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5033,7 +5032,7 @@
       </c>
       <c r="I1" s="30"/>
     </row>
-    <row r="2" spans="1:9" hidden="1">
+    <row r="2" spans="1:9">
       <c r="A2" s="24" t="s">
         <v>150</v>
       </c>
@@ -5051,7 +5050,7 @@
       </c>
       <c r="I2" s="25"/>
     </row>
-    <row r="3" spans="1:9" hidden="1">
+    <row r="3" spans="1:9">
       <c r="A3" s="24" t="s">
         <v>151</v>
       </c>
@@ -5068,7 +5067,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1">
+    <row r="4" spans="1:9">
       <c r="A4" s="24" t="s">
         <v>152</v>
       </c>
@@ -5102,7 +5101,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1">
+    <row r="6" spans="1:9">
       <c r="A6" s="24" t="s">
         <v>154</v>
       </c>
@@ -5118,7 +5117,7 @@
       <c r="G6" s="27"/>
       <c r="H6" s="27"/>
     </row>
-    <row r="7" spans="1:9" hidden="1">
+    <row r="7" spans="1:9">
       <c r="A7" s="24" t="s">
         <v>154</v>
       </c>
@@ -5135,7 +5134,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1">
+    <row r="8" spans="1:9">
       <c r="A8" s="24" t="s">
         <v>154</v>
       </c>
@@ -5152,7 +5151,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1">
+    <row r="9" spans="1:9">
       <c r="A9" s="24" t="s">
         <v>154</v>
       </c>
@@ -5169,7 +5168,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1">
+    <row r="10" spans="1:9">
       <c r="A10" s="24" t="s">
         <v>154</v>
       </c>
@@ -5186,7 +5185,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1">
+    <row r="11" spans="1:9">
       <c r="A11" s="24" t="s">
         <v>154</v>
       </c>
@@ -5206,7 +5205,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1">
+    <row r="12" spans="1:9">
       <c r="A12" s="24" t="s">
         <v>154</v>
       </c>
@@ -5339,7 +5338,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1">
+    <row r="19" spans="1:9">
       <c r="A19" s="24" t="s">
         <v>156</v>
       </c>
@@ -5355,7 +5354,7 @@
       <c r="G19" s="27"/>
       <c r="H19" s="27"/>
     </row>
-    <row r="20" spans="1:9" hidden="1">
+    <row r="20" spans="1:9">
       <c r="A20" s="24" t="s">
         <v>156</v>
       </c>
@@ -5375,7 +5374,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1">
+    <row r="21" spans="1:9">
       <c r="A21" s="24" t="s">
         <v>156</v>
       </c>
@@ -5395,7 +5394,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1">
+    <row r="22" spans="1:9">
       <c r="A22" s="24" t="s">
         <v>156</v>
       </c>
@@ -5599,7 +5598,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1">
+    <row r="33" spans="1:8">
       <c r="A33" s="24" t="s">
         <v>158</v>
       </c>
@@ -5615,7 +5614,7 @@
       <c r="G33" s="27"/>
       <c r="H33" s="27"/>
     </row>
-    <row r="34" spans="1:8" hidden="1">
+    <row r="34" spans="1:8">
       <c r="A34" s="24" t="s">
         <v>158</v>
       </c>
@@ -5635,7 +5634,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1">
+    <row r="35" spans="1:8">
       <c r="A35" s="24" t="s">
         <v>158</v>
       </c>
@@ -5655,7 +5654,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1">
+    <row r="36" spans="1:8">
       <c r="A36" s="24" t="s">
         <v>158</v>
       </c>
@@ -5675,7 +5674,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1">
+    <row r="37" spans="1:8">
       <c r="A37" s="24" t="s">
         <v>158</v>
       </c>
@@ -5695,7 +5694,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1">
+    <row r="38" spans="1:8">
       <c r="A38" s="24" t="s">
         <v>158</v>
       </c>
@@ -5715,7 +5714,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1">
+    <row r="39" spans="1:8">
       <c r="A39" s="24" t="s">
         <v>158</v>
       </c>
@@ -5735,7 +5734,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1">
+    <row r="40" spans="1:8">
       <c r="A40" s="24" t="s">
         <v>158</v>
       </c>
@@ -5755,7 +5754,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1">
+    <row r="41" spans="1:8">
       <c r="A41" s="24" t="s">
         <v>158</v>
       </c>
@@ -5775,7 +5774,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1">
+    <row r="42" spans="1:8">
       <c r="A42" s="24" t="s">
         <v>158</v>
       </c>
@@ -5795,7 +5794,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1">
+    <row r="43" spans="1:8">
       <c r="A43" s="24" t="s">
         <v>158</v>
       </c>
@@ -6001,7 +6000,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1">
+    <row r="55" spans="1:8">
       <c r="A55" s="24" t="s">
         <v>158</v>
       </c>
@@ -6017,7 +6016,7 @@
       <c r="G55" s="27"/>
       <c r="H55" s="27"/>
     </row>
-    <row r="56" spans="1:8" ht="30" hidden="1">
+    <row r="56" spans="1:8" ht="30">
       <c r="A56" s="24" t="s">
         <v>158</v>
       </c>
@@ -6037,7 +6036,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="30" hidden="1">
+    <row r="57" spans="1:8" ht="30">
       <c r="A57" s="24" t="s">
         <v>158</v>
       </c>
@@ -6057,7 +6056,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="30" hidden="1">
+    <row r="58" spans="1:8" ht="30">
       <c r="A58" s="24" t="s">
         <v>158</v>
       </c>
@@ -6077,7 +6076,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="30" hidden="1">
+    <row r="59" spans="1:8" ht="30">
       <c r="A59" s="24" t="s">
         <v>158</v>
       </c>
@@ -6097,7 +6096,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1">
+    <row r="60" spans="1:8">
       <c r="A60" s="24" t="s">
         <v>158</v>
       </c>
@@ -6117,7 +6116,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1">
+    <row r="61" spans="1:8">
       <c r="A61" s="24" t="s">
         <v>158</v>
       </c>
@@ -6137,7 +6136,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1">
+    <row r="62" spans="1:8">
       <c r="A62" s="24" t="s">
         <v>158</v>
       </c>
@@ -6157,7 +6156,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1">
+    <row r="63" spans="1:8">
       <c r="A63" s="24" t="s">
         <v>158</v>
       </c>
@@ -6178,13 +6177,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I63">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="I"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <conditionalFormatting sqref="F1:H1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Sim"</formula>

</xml_diff>